<commit_message>
update ig list rendering
</commit_message>
<xml_diff>
--- a/CapStatement/temp_source_spreadsheets/test-spreadsheet.xlsx
+++ b/CapStatement/temp_source_spreadsheets/test-spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/CapStatement/temp_source_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22DD97A-F9DA-A247-B5A0-0EF36CDA6E34}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066FAEA1-E4CB-4E41-AA89-918ABADD49DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="460" windowWidth="25200" windowHeight="13660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3500" yWindow="460" windowWidth="25200" windowHeight="13660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -33,7 +33,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -143,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="541">
   <si>
     <t>Element</t>
   </si>
@@ -1785,6 +1788,9 @@
   </si>
   <si>
     <t>http://example.org/fhir/my-allergyintolerance</t>
+  </si>
+  <si>
+    <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
   </si>
 </sst>
 </file>
@@ -4877,7 +4883,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4965,20 +4971,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.83203125" customWidth="1"/>
+    <col min="2" max="2" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -5429,7 +5454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
added primitive extension support using fhir.resources
</commit_message>
<xml_diff>
--- a/CapStatement/temp_source_spreadsheets/test-spreadsheet.xlsx
+++ b/CapStatement/temp_source_spreadsheets/test-spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/CapStatement/temp_source_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066FAEA1-E4CB-4E41-AA89-918ABADD49DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F94DDB-5494-DE45-8DC4-D31EFB6E5495}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="460" windowWidth="25200" windowHeight="13660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2440" yWindow="460" windowWidth="25200" windowHeight="13660" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sp_combos!$B$1:$B$77</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">sps!$A$1:$AB$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">sps!$A$1:$AC$94</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -117,7 +117,7 @@
     <author>User</author>
   </authors>
   <commentList>
-    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{B8B118CB-23C6-4556-9470-64A59EB595D7}">
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{B8B118CB-23C6-4556-9470-64A59EB595D7}">
       <text>
         <r>
           <rPr>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="543">
   <si>
     <t>Element</t>
   </si>
@@ -1791,6 +1791,12 @@
   </si>
   <si>
     <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>json,xml</t>
   </si>
 </sst>
 </file>
@@ -1872,6 +1878,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4880,10 +4887,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4964,6 +4971,14 @@
         <v>456</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4973,7 +4988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6070,13 +6085,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6087,13 +6102,14 @@
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="58.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="28.1640625" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" customWidth="1"/>
-    <col min="17" max="17" width="31.33203125" customWidth="1"/>
-    <col min="18" max="18" width="31.33203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="20.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" customWidth="1"/>
+    <col min="18" max="18" width="31.33203125" customWidth="1"/>
+    <col min="19" max="19" width="31.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="20.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -6118,59 +6134,59 @@
       <c r="H1" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>426</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -6195,11 +6211,8 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s">
         <v>34</v>
@@ -6222,7 +6235,7 @@
       <c r="Q2" t="s">
         <v>34</v>
       </c>
-      <c r="S2" t="s">
+      <c r="R2" t="s">
         <v>34</v>
       </c>
       <c r="T2" t="s">
@@ -6237,11 +6250,14 @@
       <c r="W2" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -6263,9 +6279,6 @@
       <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
       <c r="J3" t="s">
         <v>13</v>
       </c>
@@ -6279,10 +6292,10 @@
         <v>13</v>
       </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="O3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="P3" t="s">
         <v>13</v>
@@ -6290,10 +6303,10 @@
       <c r="Q3" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="2"/>
-      <c r="S3" t="s">
-        <v>13</v>
-      </c>
+      <c r="R3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" s="2"/>
       <c r="T3" t="s">
         <v>13</v>
       </c>
@@ -6306,11 +6319,14 @@
       <c r="W3" t="s">
         <v>13</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -6332,9 +6348,6 @@
       <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
-        <v>13</v>
-      </c>
       <c r="J4" t="s">
         <v>13</v>
       </c>
@@ -6359,7 +6372,7 @@
       <c r="Q4" t="s">
         <v>13</v>
       </c>
-      <c r="S4" t="s">
+      <c r="R4" t="s">
         <v>13</v>
       </c>
       <c r="T4" t="s">
@@ -6374,11 +6387,14 @@
       <c r="W4" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -6400,9 +6416,6 @@
       <c r="H5" t="s">
         <v>78</v>
       </c>
-      <c r="I5" t="s">
-        <v>78</v>
-      </c>
       <c r="J5" t="s">
         <v>78</v>
       </c>
@@ -6427,7 +6440,7 @@
       <c r="Q5" t="s">
         <v>78</v>
       </c>
-      <c r="S5" t="s">
+      <c r="R5" t="s">
         <v>78</v>
       </c>
       <c r="T5" t="s">
@@ -6442,11 +6455,14 @@
       <c r="W5" t="s">
         <v>78</v>
       </c>
-      <c r="X5" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -6468,9 +6484,6 @@
       <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="J6" s="1" t="s">
         <v>34</v>
       </c>
@@ -6495,7 +6508,7 @@
       <c r="Q6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="T6" s="1" t="s">
@@ -6507,14 +6520,17 @@
       <c r="V6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="W6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -6536,9 +6552,6 @@
       <c r="H7" t="s">
         <v>34</v>
       </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
       <c r="J7" t="s">
         <v>34</v>
       </c>
@@ -6563,7 +6576,7 @@
       <c r="Q7" t="s">
         <v>34</v>
       </c>
-      <c r="S7" t="s">
+      <c r="R7" t="s">
         <v>34</v>
       </c>
       <c r="T7" t="s">
@@ -6578,11 +6591,14 @@
       <c r="W7" t="s">
         <v>34</v>
       </c>
-      <c r="X7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -6604,9 +6620,6 @@
       <c r="H8" t="s">
         <v>34</v>
       </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
       <c r="J8" t="s">
         <v>34</v>
       </c>
@@ -6631,7 +6644,7 @@
       <c r="Q8" t="s">
         <v>34</v>
       </c>
-      <c r="S8" t="s">
+      <c r="R8" t="s">
         <v>34</v>
       </c>
       <c r="T8" t="s">
@@ -6646,11 +6659,14 @@
       <c r="W8" t="s">
         <v>34</v>
       </c>
-      <c r="X8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -6672,9 +6688,6 @@
       <c r="H9" t="s">
         <v>78</v>
       </c>
-      <c r="I9" t="s">
-        <v>78</v>
-      </c>
       <c r="J9" t="s">
         <v>78</v>
       </c>
@@ -6699,7 +6712,7 @@
       <c r="Q9" t="s">
         <v>78</v>
       </c>
-      <c r="S9" t="s">
+      <c r="R9" t="s">
         <v>78</v>
       </c>
       <c r="T9" t="s">
@@ -6714,11 +6727,14 @@
       <c r="W9" t="s">
         <v>78</v>
       </c>
-      <c r="X9" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X9" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -6740,9 +6756,6 @@
       <c r="H10" t="s">
         <v>34</v>
       </c>
-      <c r="I10" t="s">
-        <v>34</v>
-      </c>
       <c r="J10" t="s">
         <v>34</v>
       </c>
@@ -6767,7 +6780,7 @@
       <c r="Q10" t="s">
         <v>34</v>
       </c>
-      <c r="S10" t="s">
+      <c r="R10" t="s">
         <v>34</v>
       </c>
       <c r="T10" t="s">
@@ -6782,7 +6795,10 @@
       <c r="W10" t="s">
         <v>34</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="X10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y10" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -6858,13 +6874,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AB94"/>
+  <dimension ref="A1:AC94"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="Z50" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6877,25 +6890,26 @@
     <col min="6" max="6" width="73.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="49.6640625" style="1" customWidth="1"/>
-    <col min="21" max="22" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.1640625" customWidth="1"/>
+    <col min="11" max="11" width="36.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="49.6640625" style="1" customWidth="1"/>
+    <col min="22" max="23" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" style="1" customWidth="1"/>
+    <col min="25" max="25" width="50.83203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="90.6640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="83.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>151</v>
       </c>
@@ -6927,61 +6941,64 @@
         <v>46</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -7014,24 +7031,24 @@
         <f>B2&amp;"."&amp;C2</f>
         <v>!EXAMPLE CATEGORY SEARCH.category</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="1" t="str">
-        <f t="shared" ref="AB2:AB4" si="0">"SearchParameter-us-core-"&amp;LOWER((B2)&amp;"-"&amp;C2&amp;".html")</f>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="1" t="str">
+        <f t="shared" ref="AC2:AC4" si="0">"SearchParameter-us-core-"&amp;LOWER((B2)&amp;"-"&amp;C2&amp;".html")</f>
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -7064,21 +7081,21 @@
         <f>B3&amp;"."&amp;C3</f>
         <v>!EXAMPLE CODE SEARCH.code</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y3" s="5"/>
+      <c r="L3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="Z3" s="5"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="1" t="str">
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -7111,28 +7128,28 @@
         <f>B4&amp;"."&amp;C4</f>
         <v>!EXAMPLE DATE SEARCH.date</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="1" t="str">
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -7165,33 +7182,33 @@
         <f>B5&amp;"."&amp;C5</f>
         <v>!EXAMPLE PATIENT SEARCH.patient</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X5" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y5" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y5" s="1" t="str">
+      <c r="Z5" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B5)&amp;"s for a patient"</f>
         <v>support searching for all !example patient searchs for a patient</v>
       </c>
-      <c r="Z5" s="5" t="str">
+      <c r="AA5" s="5" t="str">
         <f>"GET [base]/"&amp;B5&amp;"?patient=1137192"</f>
         <v>GET [base]/!EXAMPLE PATIENT SEARCH?patient=1137192</v>
       </c>
-      <c r="AA5" s="12" t="str">
+      <c r="AB5" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B5&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all !EXAMPLE PATIENT SEARCH resources for the specified patient</v>
       </c>
-      <c r="AB5" s="1" t="str">
+      <c r="AC5" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B5)&amp;"-"&amp;C5&amp;".html")</f>
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -7224,24 +7241,24 @@
         <f t="shared" ref="J6" si="2">B6&amp;"."&amp;C6</f>
         <v>!EXAMPLE STATUS SEARCH.status</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X6" s="1" t="s">
+      <c r="L6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="1" t="str">
-        <f t="shared" ref="AB6" si="3">"SearchParameter-us-core-"&amp;LOWER((B6)&amp;"-"&amp;C6&amp;".html")</f>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="1" t="str">
+        <f t="shared" ref="AC6" si="3">"SearchParameter-us-core-"&amp;LOWER((B6)&amp;"-"&amp;C6&amp;".html")</f>
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -7274,25 +7291,25 @@
         <f t="shared" ref="J7:J22" si="4">B7&amp;"."&amp;C7</f>
         <v>!Patient.address</v>
       </c>
-      <c r="K7" t="s">
-        <v>62</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y7" s="1" t="s">
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z7" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="Z7" s="5" t="s">
+      <c r="AA7" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="AA7" s="12"/>
-      <c r="AB7" t="str">
+      <c r="AB7" s="12"/>
+      <c r="AC7" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B7)&amp;"-"&amp;C7&amp;".html")</f>
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -7325,25 +7342,25 @@
         <f t="shared" si="4"/>
         <v>!Patient.telecom</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y8" s="1" t="s">
+      <c r="L8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z8" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="1" t="str">
-        <f t="shared" ref="AB8:AB39" si="5">"SearchParameter-us-core-"&amp;LOWER((B8)&amp;"-"&amp;C8&amp;".html")</f>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="1" t="str">
+        <f t="shared" ref="AC8:AC39" si="5">"SearchParameter-us-core-"&amp;LOWER((B8)&amp;"-"&amp;C8&amp;".html")</f>
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -7376,21 +7393,21 @@
         <f t="shared" si="4"/>
         <v>AllergyIntolerance.clinical-status</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X9"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="12"/>
-      <c r="AB9" s="1" t="str">
+      <c r="L9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y9"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -7423,34 +7440,34 @@
         <f t="shared" si="4"/>
         <v>AllergyIntolerance.patient</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P10"/>
+      <c r="L10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="Q10"/>
-      <c r="S10"/>
+      <c r="R10"/>
       <c r="T10"/>
-      <c r="X10"/>
-      <c r="Y10" t="s">
+      <c r="U10"/>
+      <c r="Y10"/>
+      <c r="Z10" t="s">
         <v>82</v>
       </c>
-      <c r="Z10" s="5" t="str">
+      <c r="AA10" s="5" t="str">
         <f>"GET [base]/"&amp;B10&amp;"?patient=1137192"</f>
         <v>GET [base]/AllergyIntolerance?patient=1137192</v>
       </c>
-      <c r="AA10" s="12" t="str">
+      <c r="AB10" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B10&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all AllergyIntolerance resources for the specified patient</v>
       </c>
-      <c r="AB10" s="1" t="str">
+      <c r="AC10" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B10)&amp;"-"&amp;SUBSTITUTE(C10,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -7483,25 +7500,25 @@
         <f t="shared" si="4"/>
         <v>Condition.category</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O11"/>
-      <c r="X11" t="s">
+      <c r="L11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P11"/>
+      <c r="Y11" t="s">
         <v>14</v>
       </c>
-      <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="12"/>
-      <c r="AB11" s="1" t="str">
+      <c r="AA11" s="5"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -7534,22 +7551,22 @@
         <f t="shared" si="4"/>
         <v>Condition.clinical-status</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X12" s="1" t="s">
+      <c r="L12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y12" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA12" s="12"/>
-      <c r="AB12" s="1" t="str">
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -7582,32 +7599,32 @@
         <f t="shared" si="4"/>
         <v>Condition.patient</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X13" s="1" t="s">
+      <c r="L13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y13" s="1" t="s">
+      <c r="Z13" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="Z13" s="5" t="str">
+      <c r="AA13" s="5" t="str">
         <f>"GET [base]/"&amp;B13&amp;"?patient=1137192"</f>
         <v>GET [base]/Condition?patient=1137192</v>
       </c>
-      <c r="AA13" s="12" t="str">
+      <c r="AB13" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B13&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all Condition resources for the specified patient</v>
       </c>
-      <c r="AB13" s="1" t="str">
-        <f t="shared" ref="AB13:AB14" si="6">"SearchParameter-us-core-"&amp;LOWER((B13)&amp;"-"&amp;SUBSTITUTE(C13,"_","")&amp;".html")</f>
+      <c r="AC13" s="1" t="str">
+        <f t="shared" ref="AC13:AC14" si="6">"SearchParameter-us-core-"&amp;LOWER((B13)&amp;"-"&amp;SUBSTITUTE(C13,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -7640,27 +7657,27 @@
         <f t="shared" si="4"/>
         <v>Encounter._id</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y14" s="5" t="s">
+      <c r="L14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z14" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="Z14" s="5" t="s">
+      <c r="AA14" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="AA14" s="2" t="s">
+      <c r="AB14" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AB14" s="1" t="str">
+      <c r="AC14" s="1" t="str">
         <f t="shared" si="6"/>
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -7693,24 +7710,24 @@
         <f t="shared" si="4"/>
         <v>Encounter.class</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X15" s="1" t="s">
+      <c r="L15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
-      <c r="AA15" s="12"/>
-      <c r="AB15" s="1" t="str">
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="12"/>
+      <c r="AC15" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -7743,28 +7760,28 @@
         <f t="shared" si="4"/>
         <v>Encounter.date</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X16" s="1" t="s">
+      <c r="Y16" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="1" t="str">
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -7797,28 +7814,28 @@
         <f t="shared" si="4"/>
         <v>Encounter.identifier</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y17" s="5" t="s">
+      <c r="L17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z17" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>171</v>
       </c>
-      <c r="AA17" s="12" t="str">
+      <c r="AB17" s="12" t="str">
         <f>"Fetches a bundle containing any "&amp;B17&amp;" resources matching the identifier"</f>
         <v>Fetches a bundle containing any Encounter resources matching the identifier</v>
       </c>
-      <c r="AB17" s="1" t="str">
-        <f t="shared" ref="AB17:AB18" si="7">"SearchParameter-us-core-"&amp;LOWER((B17)&amp;"-"&amp;SUBSTITUTE(C17,"_","")&amp;".html")</f>
+      <c r="AC17" s="1" t="str">
+        <f t="shared" ref="AC17:AC18" si="7">"SearchParameter-us-core-"&amp;LOWER((B17)&amp;"-"&amp;SUBSTITUTE(C17,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -7851,32 +7868,32 @@
         <f t="shared" si="4"/>
         <v>Encounter.patient</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X18" t="s">
+      <c r="L18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y18" t="s">
         <v>101</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>102</v>
       </c>
-      <c r="Z18" s="5" t="str">
+      <c r="AA18" s="5" t="str">
         <f>"GET [base]/"&amp;B18&amp;"?patient=1137192"</f>
         <v>GET [base]/Encounter?patient=1137192</v>
       </c>
-      <c r="AA18" s="12" t="str">
+      <c r="AB18" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B18&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all Encounter resources for the specified patient</v>
       </c>
-      <c r="AB18" s="1" t="str">
+      <c r="AC18" s="1" t="str">
         <f t="shared" si="7"/>
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -7909,24 +7926,24 @@
         <f t="shared" si="4"/>
         <v>Encounter.status</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X19" t="s">
+      <c r="L19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y19" t="s">
         <v>104</v>
       </c>
-      <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
-      <c r="AA19" s="12"/>
-      <c r="AB19" s="1" t="str">
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -7959,22 +7976,22 @@
         <f t="shared" si="4"/>
         <v>Encounter.type</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X20"/>
-      <c r="Y20" s="5"/>
+      <c r="L20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y20"/>
       <c r="Z20" s="5"/>
-      <c r="AA20" s="12"/>
-      <c r="AB20" s="1" t="str">
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="12"/>
+      <c r="AC20" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -8007,24 +8024,24 @@
         <f t="shared" si="4"/>
         <v>Patient._id</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y21" s="5" t="s">
+      <c r="L21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z21" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="Z21" s="5" t="s">
+      <c r="AA21" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="AB21" s="1" t="str">
+      <c r="AC21" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B21)&amp;"-"&amp;SUBSTITUTE(C21,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -8057,22 +8074,22 @@
         <f t="shared" si="4"/>
         <v>Patient.birthdate</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X22" s="1" t="s">
+      <c r="L22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="Z22"/>
-      <c r="AB22" s="1" t="str">
+      <c r="AA22"/>
+      <c r="AC22" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -8104,19 +8121,20 @@
       <c r="J23" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y23"/>
-      <c r="AB23" s="1" t="str">
+      <c r="K23" s="6"/>
+      <c r="L23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z23"/>
+      <c r="AC23" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -8149,23 +8167,23 @@
         <f>B24&amp;"."&amp;C24</f>
         <v>Patient.gender</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X24" s="1" t="s">
+      <c r="L24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y24" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="Y24"/>
-      <c r="AA24" s="12"/>
-      <c r="AB24" s="1" t="str">
+      <c r="Z24"/>
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -8197,19 +8215,20 @@
       <c r="J25" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA25" s="12"/>
-      <c r="AB25" s="1" t="str">
+      <c r="K25" s="6"/>
+      <c r="L25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB25" s="12"/>
+      <c r="AC25" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -8242,29 +8261,29 @@
         <f>B26&amp;"."&amp;C26</f>
         <v>Patient.identifier</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X26"/>
-      <c r="Y26" s="5" t="s">
+      <c r="L26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y26"/>
+      <c r="Z26" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="Z26" s="1" t="s">
+      <c r="AA26" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AA26" s="12" t="str">
+      <c r="AB26" s="12" t="str">
         <f>"Fetches a bundle containing any "&amp;B26&amp;" resources matching the identifier"</f>
         <v>Fetches a bundle containing any Patient resources matching the identifier</v>
       </c>
-      <c r="AB26" s="1" t="str">
-        <f t="shared" ref="AB26:AB27" si="8">"SearchParameter-us-core-"&amp;LOWER((B26)&amp;"-"&amp;SUBSTITUTE(C26,"_","")&amp;".html")</f>
+      <c r="AC26" s="1" t="str">
+        <f t="shared" ref="AC26:AC27" si="8">"SearchParameter-us-core-"&amp;LOWER((B26)&amp;"-"&amp;SUBSTITUTE(C26,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -8297,32 +8316,32 @@
         <f>B27&amp;"."&amp;C27</f>
         <v>Patient.name</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q27"/>
-      <c r="X27" t="s">
+      <c r="L27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R27"/>
+      <c r="Y27" t="s">
         <v>86</v>
       </c>
-      <c r="Y27" s="5" t="s">
+      <c r="Z27" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="Z27" s="1" t="s">
+      <c r="AA27" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AA27" s="12" t="str">
+      <c r="AB27" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B27&amp;" resources matching the name"</f>
         <v>Fetches a bundle of all Patient resources matching the name</v>
       </c>
-      <c r="AB27" s="1" t="str">
+      <c r="AC27" s="1" t="str">
         <f t="shared" si="8"/>
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -8354,18 +8373,18 @@
       <c r="J28" t="s">
         <v>64</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB28" s="1" t="str">
+      <c r="L28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC28" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -8398,19 +8417,19 @@
         <f t="shared" ref="J29:J39" si="9">B29&amp;"."&amp;C29</f>
         <v>!Questionnaire.context-type-value</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X29"/>
-      <c r="AB29" s="1" t="str">
+      <c r="L29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y29"/>
+      <c r="AC29" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -8443,24 +8462,24 @@
         <f t="shared" si="9"/>
         <v>!Questionnaire.publisher</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O30" s="1" t="s">
+      <c r="L30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="X30" t="s">
+      <c r="Y30" t="s">
         <v>77</v>
       </c>
-      <c r="AB30" s="1" t="str">
+      <c r="AC30" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -8493,21 +8512,21 @@
         <f t="shared" si="9"/>
         <v>!Questionnaire.status</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X31" s="1" t="s">
+      <c r="L31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y31" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AB31" s="1" t="str">
+      <c r="AC31" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -8540,34 +8559,34 @@
         <f t="shared" si="9"/>
         <v>!Questionnaire.title</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P32" s="1" t="s">
+      <c r="L32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="R32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="S32" s="1" t="s">
+      <c r="T32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T32" s="1" t="s">
+      <c r="U32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="X32" s="1" t="s">
+      <c r="Y32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AA32" s="2"/>
-      <c r="AB32" s="1" t="str">
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -8600,19 +8619,19 @@
         <f t="shared" si="9"/>
         <v>!Questionnaire.url</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA33" s="2"/>
-      <c r="AB33" s="1" t="str">
+      <c r="L33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -8645,19 +8664,19 @@
         <f t="shared" si="9"/>
         <v>!Questionnaire.version</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA34" s="2"/>
-      <c r="AB34" s="1" t="str">
+      <c r="L34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -8690,25 +8709,25 @@
         <f t="shared" si="9"/>
         <v>Condition.onset-date</v>
       </c>
-      <c r="K35" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AA35" s="12"/>
-      <c r="AB35" s="1" t="str">
+      <c r="AB35" s="12"/>
+      <c r="AC35" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -8741,21 +8760,21 @@
         <f t="shared" si="9"/>
         <v>Condition.code</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y36" s="5"/>
+      <c r="L36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="Z36" s="5"/>
-      <c r="AA36" s="12"/>
-      <c r="AB36" s="1" t="str">
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="12"/>
+      <c r="AC36" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -8788,33 +8807,33 @@
         <f t="shared" si="9"/>
         <v>Immunization.patient</v>
       </c>
-      <c r="K37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X37" s="1" t="s">
+      <c r="L37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y37" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y37" s="1" t="str">
+      <c r="Z37" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B37)&amp;"s for a patient"</f>
         <v>support searching for all immunizations for a patient</v>
       </c>
-      <c r="Z37" s="5" t="str">
+      <c r="AA37" s="5" t="str">
         <f>"GET [base]/"&amp;B37&amp;"?patient=1137192"</f>
         <v>GET [base]/Immunization?patient=1137192</v>
       </c>
-      <c r="AA37" s="12" t="str">
+      <c r="AB37" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B37&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all Immunization resources for the specified patient</v>
       </c>
-      <c r="AB37" s="1" t="str">
+      <c r="AC37" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B37)&amp;"-"&amp;SUBSTITUTE(C37,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -8847,24 +8866,24 @@
         <f t="shared" si="9"/>
         <v>Immunization.status</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X38" s="1" t="s">
+      <c r="L38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y38" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
-      <c r="AA38" s="12"/>
-      <c r="AB38" s="1" t="str">
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="12"/>
+      <c r="AC38" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -8897,28 +8916,28 @@
         <f t="shared" si="9"/>
         <v>Immunization.date</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R39" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X39" s="1" t="s">
+      <c r="Y39" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA39" s="12"/>
-      <c r="AB39" s="1" t="str">
+      <c r="AB39" s="12"/>
+      <c r="AC39" s="1" t="str">
         <f t="shared" si="5"/>
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -8951,27 +8970,27 @@
         <f>B40&amp;".id"</f>
         <v>DocumentReference.id</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y40" s="5" t="s">
+      <c r="L40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z40" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="Z40" s="5" t="s">
+      <c r="AA40" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="AA40" s="2" t="s">
+      <c r="AB40" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="AB40" s="1" t="str">
-        <f t="shared" ref="AB40" si="10">"SearchParameter-us-core-"&amp;LOWER((B40)&amp;"-"&amp;C40&amp;".html")</f>
+      <c r="AC40" s="1" t="str">
+        <f t="shared" ref="AC40" si="10">"SearchParameter-us-core-"&amp;LOWER((B40)&amp;"-"&amp;C40&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -9004,27 +9023,27 @@
         <f t="shared" ref="J41:J67" si="11">B41&amp;"."&amp;C41</f>
         <v>DocumentReference.status</v>
       </c>
-      <c r="K41" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L41" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y41" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
-      <c r="AA41" s="12"/>
-      <c r="AB41" s="1" t="str">
-        <f t="shared" ref="AB41:AB70" si="12">"SearchParameter-us-core-"&amp;LOWER((B41)&amp;"-"&amp;C41&amp;".html")</f>
+      <c r="AA41" s="5"/>
+      <c r="AB41" s="12"/>
+      <c r="AC41" s="1" t="str">
+        <f t="shared" ref="AC41:AC70" si="12">"SearchParameter-us-core-"&amp;LOWER((B41)&amp;"-"&amp;C41&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -9057,33 +9076,33 @@
         <f t="shared" si="11"/>
         <v>DocumentReference.patient</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X42" s="1" t="s">
+      <c r="L42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y42" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y42" s="1" t="str">
+      <c r="Z42" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B42)&amp;"s for a patient"</f>
         <v>support searching for all documentreferences for a patient</v>
       </c>
-      <c r="Z42" s="5" t="str">
+      <c r="AA42" s="5" t="str">
         <f>"GET [base]/"&amp;B42&amp;"?patient=1137192"</f>
         <v>GET [base]/DocumentReference?patient=1137192</v>
       </c>
-      <c r="AA42" s="12" t="str">
+      <c r="AB42" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B42&amp; " resources for the specified patient. See the implementation notes above for how to access the actual document."</f>
         <v>Fetches a bundle of all DocumentReference resources for the specified patient. See the implementation notes above for how to access the actual document.</v>
       </c>
-      <c r="AB42" s="1" t="str">
-        <f t="shared" ref="AB42:AB45" si="13">"SearchParameter-us-core-"&amp;LOWER((B42)&amp;"-"&amp;C42&amp;".html")</f>
+      <c r="AC42" s="1" t="str">
+        <f t="shared" ref="AC42:AC45" si="13">"SearchParameter-us-core-"&amp;LOWER((B42)&amp;"-"&amp;C42&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -9116,24 +9135,24 @@
         <f t="shared" ref="J43:J45" si="14">B43&amp;"."&amp;C43</f>
         <v>DocumentReference.category</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X43" s="1" t="s">
+      <c r="L43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y43" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
-      <c r="AA43" s="12"/>
-      <c r="AB43" s="1" t="str">
+      <c r="AA43" s="5"/>
+      <c r="AB43" s="12"/>
+      <c r="AC43" s="1" t="str">
         <f t="shared" si="13"/>
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -9166,21 +9185,21 @@
         <f t="shared" si="14"/>
         <v>DocumentReference.type</v>
       </c>
-      <c r="K44" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y44" s="5"/>
+      <c r="L44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="Z44" s="5"/>
-      <c r="AA44" s="12"/>
-      <c r="AB44" s="1" t="str">
+      <c r="AA44" s="5"/>
+      <c r="AB44" s="12"/>
+      <c r="AC44" s="1" t="str">
         <f t="shared" si="13"/>
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -9213,28 +9232,28 @@
         <f t="shared" si="14"/>
         <v>DocumentReference.date</v>
       </c>
-      <c r="K45" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R45" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X45" s="1" t="s">
+      <c r="Y45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA45" s="12"/>
-      <c r="AB45" s="1" t="str">
+      <c r="AB45" s="12"/>
+      <c r="AC45" s="1" t="str">
         <f t="shared" si="13"/>
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -9266,28 +9285,28 @@
       <c r="J46" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="K46" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M46" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q46" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R46" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X46" s="1" t="s">
+      <c r="Y46" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA46" s="12"/>
-      <c r="AB46" s="1" t="str">
-        <f t="shared" ref="AB46" si="15">"SearchParameter-us-core-"&amp;LOWER((B46)&amp;"-"&amp;C46&amp;".html")</f>
+      <c r="AB46" s="12"/>
+      <c r="AC46" s="1" t="str">
+        <f t="shared" ref="AC46" si="15">"SearchParameter-us-core-"&amp;LOWER((B46)&amp;"-"&amp;C46&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -9320,27 +9339,27 @@
         <f t="shared" ref="J47:J51" si="16">B47&amp;"."&amp;C47</f>
         <v>DiagnosticReport.status</v>
       </c>
-      <c r="K47" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L47" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y47" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y47" s="5"/>
       <c r="Z47" s="5"/>
-      <c r="AA47" s="12"/>
-      <c r="AB47" s="1" t="str">
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="12"/>
+      <c r="AC47" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B47)&amp;"-"&amp;C47&amp;".html")</f>
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -9373,33 +9392,33 @@
         <f t="shared" si="16"/>
         <v>DiagnosticReport.patient</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X48" s="1" t="s">
+      <c r="L48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y48" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y48" s="1" t="str">
+      <c r="Z48" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B48)&amp;"s for a patient"</f>
         <v>support searching for all diagnosticreports for a patient</v>
       </c>
-      <c r="Z48" s="5" t="str">
+      <c r="AA48" s="5" t="str">
         <f>"GET [base]/"&amp;B48&amp;"?patient=1137192"</f>
         <v>GET [base]/DiagnosticReport?patient=1137192</v>
       </c>
-      <c r="AA48" s="12" t="str">
+      <c r="AB48" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B48&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient</v>
       </c>
-      <c r="AB48" s="1" t="str">
+      <c r="AC48" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B48)&amp;"-"&amp;C48&amp;".html")</f>
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -9432,24 +9451,24 @@
         <f t="shared" si="16"/>
         <v>DiagnosticReport.category</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X49" s="1" t="s">
+      <c r="L49" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y49" s="5"/>
       <c r="Z49" s="5"/>
-      <c r="AA49" s="12"/>
-      <c r="AB49" s="1" t="str">
+      <c r="AA49" s="5"/>
+      <c r="AB49" s="12"/>
+      <c r="AC49" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B49)&amp;"-"&amp;C49&amp;".html")</f>
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -9482,24 +9501,24 @@
         <f t="shared" si="16"/>
         <v>DiagnosticReport.code</v>
       </c>
-      <c r="K50" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L50" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y50" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="Z50" s="5"/>
-      <c r="AA50" s="12"/>
-      <c r="AB50" s="1" t="str">
+      <c r="AA50" s="5"/>
+      <c r="AB50" s="12"/>
+      <c r="AC50" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B50)&amp;"-"&amp;C50&amp;".html")</f>
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -9532,28 +9551,28 @@
         <f t="shared" si="16"/>
         <v>DiagnosticReport.date</v>
       </c>
-      <c r="K51" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N51" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q51" s="1" t="s">
+      <c r="L51" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O51" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="R51" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X51" s="1" t="s">
+      <c r="Y51" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA51" s="12"/>
-      <c r="AB51" s="1" t="str">
+      <c r="AB51" s="12"/>
+      <c r="AC51" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B51)&amp;"-"&amp;C51&amp;".html")</f>
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -9586,24 +9605,24 @@
         <f t="shared" si="11"/>
         <v>Goal.lifecycle-status</v>
       </c>
-      <c r="K52" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X52" s="1" t="s">
+      <c r="L52" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y52" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y52" s="5"/>
       <c r="Z52" s="5"/>
-      <c r="AA52" s="12"/>
-      <c r="AB52" s="1" t="str">
+      <c r="AA52" s="5"/>
+      <c r="AB52" s="12"/>
+      <c r="AC52" s="1" t="str">
         <f t="shared" si="12"/>
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -9636,33 +9655,33 @@
         <f t="shared" si="11"/>
         <v>Goal.patient</v>
       </c>
-      <c r="K53" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X53" s="1" t="s">
+      <c r="L53" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y53" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y53" s="1" t="str">
+      <c r="Z53" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B53)&amp;"s for a patient"</f>
         <v>support searching for all goals for a patient</v>
       </c>
-      <c r="Z53" s="5" t="str">
+      <c r="AA53" s="5" t="str">
         <f>"GET [base]/"&amp;B53&amp;"?patient=1137192"</f>
         <v>GET [base]/Goal?patient=1137192</v>
       </c>
-      <c r="AA53" s="12" t="str">
+      <c r="AB53" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B53&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all Goal resources for the specified patient</v>
       </c>
-      <c r="AB53" s="1" t="str">
-        <f t="shared" ref="AB53:AB54" si="17">"SearchParameter-us-core-"&amp;LOWER((B53)&amp;"-"&amp;C53&amp;".html")</f>
+      <c r="AC53" s="1" t="str">
+        <f t="shared" ref="AC53:AC54" si="17">"SearchParameter-us-core-"&amp;LOWER((B53)&amp;"-"&amp;C53&amp;".html")</f>
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -9695,28 +9714,28 @@
         <f t="shared" ref="J54" si="18">B54&amp;"."&amp;C54</f>
         <v>Goal.target-date</v>
       </c>
-      <c r="K54" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M54" s="1" t="s">
+      <c r="L54" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q54" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R54" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X54" s="1" t="s">
+      <c r="Y54" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA54" s="12"/>
-      <c r="AB54" s="1" t="str">
+      <c r="AB54" s="12"/>
+      <c r="AC54" s="1" t="str">
         <f t="shared" si="17"/>
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -9749,27 +9768,27 @@
         <f t="shared" si="11"/>
         <v>MedicationRequest.status</v>
       </c>
-      <c r="K55" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L55" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y55" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y55" s="5"/>
       <c r="Z55" s="5"/>
-      <c r="AA55" s="12"/>
-      <c r="AB55" s="1" t="str">
+      <c r="AA55" s="5"/>
+      <c r="AB55" s="12"/>
+      <c r="AC55" s="1" t="str">
         <f t="shared" si="12"/>
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>53</v>
       </c>
@@ -9802,27 +9821,27 @@
         <f t="shared" ref="J56" si="19">B56&amp;"."&amp;C56</f>
         <v>MedicationRequest.intent</v>
       </c>
-      <c r="K56" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L56" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y56" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y56" s="5"/>
       <c r="Z56" s="5"/>
-      <c r="AA56" s="12"/>
-      <c r="AB56" s="1" t="str">
-        <f t="shared" ref="AB56" si="20">"SearchParameter-us-core-"&amp;LOWER((B56)&amp;"-"&amp;C56&amp;".html")</f>
+      <c r="AA56" s="5"/>
+      <c r="AB56" s="12"/>
+      <c r="AC56" s="1" t="str">
+        <f t="shared" ref="AC56" si="20">"SearchParameter-us-core-"&amp;LOWER((B56)&amp;"-"&amp;C56&amp;".html")</f>
         <v>SearchParameter-us-core-medicationrequest-intent.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>54</v>
       </c>
@@ -9855,25 +9874,25 @@
         <f t="shared" si="11"/>
         <v>MedicationRequest.patient</v>
       </c>
-      <c r="K57" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U57" s="7"/>
+      <c r="L57" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="V57" s="7"/>
-      <c r="X57" s="1" t="s">
+      <c r="W57" s="7"/>
+      <c r="Y57" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Z57" s="12"/>
       <c r="AA57" s="12"/>
-      <c r="AB57" s="1" t="str">
-        <f t="shared" ref="AB57" si="21">"SearchParameter-us-core-"&amp;LOWER((B57)&amp;"-"&amp;C57&amp;".html")</f>
+      <c r="AB57" s="12"/>
+      <c r="AC57" s="1" t="str">
+        <f t="shared" ref="AC57" si="21">"SearchParameter-us-core-"&amp;LOWER((B57)&amp;"-"&amp;C57&amp;".html")</f>
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -9906,25 +9925,25 @@
         <f t="shared" ref="J58" si="22">B58&amp;"."&amp;C58</f>
         <v>MedicationRequest.encounter</v>
       </c>
-      <c r="K58" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="U58" s="7"/>
+      <c r="L58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="V58" s="7"/>
-      <c r="X58" s="1" t="s">
+      <c r="W58" s="7"/>
+      <c r="Y58" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Z58" s="12"/>
       <c r="AA58" s="12"/>
-      <c r="AB58" s="1" t="str">
-        <f t="shared" ref="AB58" si="23">"SearchParameter-us-core-"&amp;LOWER((B58)&amp;"-"&amp;C58&amp;".html")</f>
+      <c r="AB58" s="12"/>
+      <c r="AC58" s="1" t="str">
+        <f t="shared" ref="AC58" si="23">"SearchParameter-us-core-"&amp;LOWER((B58)&amp;"-"&amp;C58&amp;".html")</f>
         <v>SearchParameter-us-core-medicationrequest-encounter.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -9957,28 +9976,28 @@
         <f t="shared" ref="J59" si="24">B59&amp;"."&amp;C59</f>
         <v>MedicationRequest.authoredon</v>
       </c>
-      <c r="K59" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M59" s="1" t="s">
+      <c r="L59" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q59" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R59" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X59" s="1" t="s">
+      <c r="Y59" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA59" s="12"/>
-      <c r="AB59" s="1" t="str">
+      <c r="AB59" s="12"/>
+      <c r="AC59" s="1" t="str">
         <f t="shared" si="12"/>
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -10011,27 +10030,27 @@
         <f>B60&amp;"."&amp;C60</f>
         <v>!MedicationStatement.status</v>
       </c>
-      <c r="K60" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L60" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y60" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y60" s="5"/>
       <c r="Z60" s="5"/>
-      <c r="AA60" s="12"/>
-      <c r="AB60" s="1" t="str">
+      <c r="AA60" s="5"/>
+      <c r="AB60" s="12"/>
+      <c r="AC60" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B60)&amp;"-"&amp;C60&amp;".html")</f>
         <v>SearchParameter-us-core-!medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>57</v>
       </c>
@@ -10064,32 +10083,32 @@
         <f t="shared" si="11"/>
         <v>!MedicationStatement.patient</v>
       </c>
-      <c r="K61" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="V61" s="7"/>
-      <c r="X61" s="1" t="s">
+      <c r="L61" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W61" s="7"/>
+      <c r="Y61" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y61" s="1" t="s">
+      <c r="Z61" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="Z61" s="12" t="s">
+      <c r="AA61" s="12" t="s">
         <v>368</v>
       </c>
-      <c r="AA61" s="12" t="str">
+      <c r="AB61" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B61&amp; " resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter.</v>
       </c>
-      <c r="AB61" s="1" t="str">
-        <f t="shared" ref="AB61:AB62" si="25">"SearchParameter-us-core-"&amp;LOWER((B61)&amp;"-"&amp;C61&amp;".html")</f>
+      <c r="AC61" s="1" t="str">
+        <f t="shared" ref="AC61:AC62" si="25">"SearchParameter-us-core-"&amp;LOWER((B61)&amp;"-"&amp;C61&amp;".html")</f>
         <v>SearchParameter-us-core-!medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>58</v>
       </c>
@@ -10122,28 +10141,28 @@
         <f t="shared" ref="J62" si="26">B62&amp;"."&amp;C62</f>
         <v>!MedicationStatement.effective</v>
       </c>
-      <c r="K62" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N62" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q62" s="1" t="s">
+      <c r="L62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O62" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="R62" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X62" s="1" t="s">
+      <c r="Y62" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA62" s="12"/>
-      <c r="AB62" s="1" t="str">
+      <c r="AB62" s="12"/>
+      <c r="AC62" s="1" t="str">
         <f t="shared" si="25"/>
         <v>SearchParameter-us-core-!medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -10176,27 +10195,27 @@
         <f t="shared" si="11"/>
         <v>Procedure.status</v>
       </c>
-      <c r="K63" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L63" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y63" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y63" s="5"/>
       <c r="Z63" s="5"/>
-      <c r="AA63" s="12"/>
-      <c r="AB63" s="1" t="str">
+      <c r="AA63" s="5"/>
+      <c r="AB63" s="12"/>
+      <c r="AC63" s="1" t="str">
         <f t="shared" si="12"/>
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -10229,32 +10248,32 @@
         <f t="shared" si="11"/>
         <v>Procedure.patient</v>
       </c>
-      <c r="K64" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M64" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X64" s="1" t="s">
+      <c r="L64" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y64" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y64" s="1" t="str">
+      <c r="Z64" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B64)&amp;"s for a patient"</f>
         <v>support searching for all procedures for a patient</v>
       </c>
-      <c r="Z64" s="5" t="s">
+      <c r="AA64" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="AA64" s="12" t="str">
+      <c r="AB64" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all Procedure resources for the specified patient</v>
       </c>
-      <c r="AB64" s="1" t="str">
-        <f t="shared" ref="AB64:AB66" si="27">"SearchParameter-us-core-"&amp;LOWER((B64)&amp;"-"&amp;C64&amp;".html")</f>
+      <c r="AC64" s="1" t="str">
+        <f t="shared" ref="AC64:AC66" si="27">"SearchParameter-us-core-"&amp;LOWER((B64)&amp;"-"&amp;C64&amp;".html")</f>
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>61</v>
       </c>
@@ -10287,28 +10306,28 @@
         <f t="shared" ref="J65:J66" si="28">B65&amp;"."&amp;C65</f>
         <v>Procedure.date</v>
       </c>
-      <c r="K65" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M65" s="1" t="s">
+      <c r="L65" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q65" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R65" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X65" s="1" t="s">
+      <c r="Y65" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA65" s="12"/>
-      <c r="AB65" s="1" t="str">
+      <c r="AB65" s="12"/>
+      <c r="AC65" s="1" t="str">
         <f t="shared" si="27"/>
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>62</v>
       </c>
@@ -10341,24 +10360,24 @@
         <f t="shared" si="28"/>
         <v>Procedure.code</v>
       </c>
-      <c r="K66" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L66" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y66" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="N66" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="Z66" s="5"/>
-      <c r="AA66" s="12"/>
-      <c r="AB66" s="1" t="str">
+      <c r="AA66" s="5"/>
+      <c r="AB66" s="12"/>
+      <c r="AC66" s="1" t="str">
         <f t="shared" si="27"/>
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>63</v>
       </c>
@@ -10391,27 +10410,27 @@
         <f t="shared" si="11"/>
         <v>Observation.status</v>
       </c>
-      <c r="K67" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L67" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y67" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y67" s="5"/>
       <c r="Z67" s="5"/>
-      <c r="AA67" s="12"/>
-      <c r="AB67" s="1" t="str">
+      <c r="AA67" s="5"/>
+      <c r="AB67" s="12"/>
+      <c r="AC67" s="1" t="str">
         <f t="shared" si="12"/>
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>64</v>
       </c>
@@ -10444,24 +10463,24 @@
         <f t="shared" ref="J68:J70" si="30">B68&amp;"."&amp;C68</f>
         <v>Observation.category</v>
       </c>
-      <c r="K68" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M68" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X68" s="1" t="s">
+      <c r="L68" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y68" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y68" s="5"/>
       <c r="Z68" s="5"/>
-      <c r="AA68" s="12"/>
-      <c r="AB68" s="1" t="str">
+      <c r="AA68" s="5"/>
+      <c r="AB68" s="12"/>
+      <c r="AC68" s="1" t="str">
         <f t="shared" si="12"/>
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>65</v>
       </c>
@@ -10494,24 +10513,24 @@
         <f t="shared" si="30"/>
         <v>Observation.code</v>
       </c>
-      <c r="K69" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L69" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y69" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="N69" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="Z69" s="5"/>
-      <c r="AA69" s="12"/>
-      <c r="AB69" s="1" t="str">
+      <c r="AA69" s="5"/>
+      <c r="AB69" s="12"/>
+      <c r="AC69" s="1" t="str">
         <f t="shared" si="12"/>
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>66</v>
       </c>
@@ -10544,28 +10563,28 @@
         <f t="shared" si="30"/>
         <v>Observation.date</v>
       </c>
-      <c r="K70" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M70" s="1" t="s">
+      <c r="L70" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q70" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O70" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R70" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X70" s="1" t="s">
+      <c r="Y70" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA70" s="12"/>
-      <c r="AB70" s="1" t="str">
+      <c r="AB70" s="12"/>
+      <c r="AC70" s="1" t="str">
         <f t="shared" si="12"/>
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>67</v>
       </c>
@@ -10598,33 +10617,33 @@
         <f>B71&amp;"."&amp;C71</f>
         <v>Observation.patient</v>
       </c>
-      <c r="K71" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M71" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X71" s="1" t="s">
+      <c r="L71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y71" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y71" s="1" t="str">
+      <c r="Z71" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B71)&amp;"s for a patient"</f>
         <v>support searching for all observations for a patient</v>
       </c>
-      <c r="Z71" s="5" t="str">
+      <c r="AA71" s="5" t="str">
         <f>"GET [base]/"&amp;B71&amp;"?patient=1137192"</f>
         <v>GET [base]/Observation?patient=1137192</v>
       </c>
-      <c r="AA71" s="12" t="str">
+      <c r="AB71" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all Observation resources for the specified patient</v>
       </c>
-      <c r="AB71" s="1" t="str">
+      <c r="AC71" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B71)&amp;"-"&amp;C71&amp;".html")</f>
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>68</v>
       </c>
@@ -10657,24 +10676,24 @@
         <f t="shared" ref="J72:J74" si="31">B72&amp;"."&amp;C72</f>
         <v>CarePlan.category</v>
       </c>
-      <c r="K72" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M72" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X72" s="1" t="s">
+      <c r="L72" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N72" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y72" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y72" s="5"/>
       <c r="Z72" s="5"/>
-      <c r="AA72" s="12"/>
-      <c r="AB72" s="1" t="str">
-        <f t="shared" ref="AB72:AB74" si="32">"SearchParameter-us-core-"&amp;LOWER((B72)&amp;"-"&amp;C72&amp;".html")</f>
+      <c r="AA72" s="5"/>
+      <c r="AB72" s="12"/>
+      <c r="AC72" s="1" t="str">
+        <f t="shared" ref="AC72:AC74" si="32">"SearchParameter-us-core-"&amp;LOWER((B72)&amp;"-"&amp;C72&amp;".html")</f>
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>69</v>
       </c>
@@ -10707,21 +10726,21 @@
         <f t="shared" si="31"/>
         <v>!CarePlan.code</v>
       </c>
-      <c r="K73" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M73" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y73" s="5"/>
+      <c r="L73" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N73" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="Z73" s="5"/>
-      <c r="AA73" s="12"/>
-      <c r="AB73" s="1" t="str">
+      <c r="AA73" s="5"/>
+      <c r="AB73" s="12"/>
+      <c r="AC73" s="1" t="str">
         <f t="shared" si="32"/>
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>70</v>
       </c>
@@ -10754,28 +10773,28 @@
         <f t="shared" si="31"/>
         <v>CarePlan.date</v>
       </c>
-      <c r="K74" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M74" s="1" t="s">
+      <c r="L74" s="1" t="s">
         <v>62</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q74" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R74" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="X74" s="1" t="s">
+      <c r="Y74" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AA74" s="12"/>
-      <c r="AB74" s="1" t="str">
+      <c r="AB74" s="12"/>
+      <c r="AC74" s="1" t="str">
         <f t="shared" si="32"/>
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>71</v>
       </c>
@@ -10808,33 +10827,33 @@
         <f>B75&amp;"."&amp;C75</f>
         <v>CarePlan.patient</v>
       </c>
-      <c r="K75" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M75" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X75" s="1" t="s">
+      <c r="L75" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y75" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y75" s="1" t="str">
+      <c r="Z75" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B75)&amp;"s for a patient"</f>
         <v>support searching for all careplans for a patient</v>
       </c>
-      <c r="Z75" s="5" t="str">
+      <c r="AA75" s="5" t="str">
         <f>"GET [base]/"&amp;B75&amp;"?patient=1137192"</f>
         <v>GET [base]/CarePlan?patient=1137192</v>
       </c>
-      <c r="AA75" s="12" t="str">
+      <c r="AB75" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B75&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all CarePlan resources for the specified patient</v>
       </c>
-      <c r="AB75" s="1" t="str">
+      <c r="AC75" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B75)&amp;"-"&amp;C75&amp;".html")</f>
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -10867,27 +10886,27 @@
         <f t="shared" ref="J76" si="33">B76&amp;"."&amp;C76</f>
         <v>CarePlan.status</v>
       </c>
-      <c r="K76" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L76" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y76" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y76" s="5"/>
       <c r="Z76" s="5"/>
-      <c r="AA76" s="12"/>
-      <c r="AB76" s="1" t="str">
-        <f t="shared" ref="AB76" si="34">"SearchParameter-us-core-"&amp;LOWER((B76)&amp;"-"&amp;C76&amp;".html")</f>
+      <c r="AA76" s="5"/>
+      <c r="AB76" s="12"/>
+      <c r="AC76" s="1" t="str">
+        <f t="shared" ref="AC76" si="34">"SearchParameter-us-core-"&amp;LOWER((B76)&amp;"-"&amp;C76&amp;".html")</f>
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>73</v>
       </c>
@@ -10920,33 +10939,33 @@
         <f>B77&amp;"."&amp;C77</f>
         <v>CareTeam.patient</v>
       </c>
-      <c r="K77" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M77" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X77" s="1" t="s">
+      <c r="L77" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N77" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y77" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y77" s="1" t="str">
+      <c r="Z77" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B77)&amp;"s for a patient"</f>
         <v>support searching for all careteams for a patient</v>
       </c>
-      <c r="Z77" s="5" t="str">
+      <c r="AA77" s="5" t="str">
         <f>"GET [base]/"&amp;B77&amp;"?patient=1137192"</f>
         <v>GET [base]/CareTeam?patient=1137192</v>
       </c>
-      <c r="AA77" s="12" t="str">
+      <c r="AB77" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B77&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all CareTeam resources for the specified patient</v>
       </c>
-      <c r="AB77" s="1" t="str">
+      <c r="AC77" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B77)&amp;"-"&amp;C77&amp;".html")</f>
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>74</v>
       </c>
@@ -10979,27 +10998,27 @@
         <f t="shared" ref="J78" si="35">B78&amp;"."&amp;C78</f>
         <v>CareTeam.status</v>
       </c>
-      <c r="K78" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="L78" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y78" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="Y78" s="5"/>
       <c r="Z78" s="5"/>
-      <c r="AA78" s="12"/>
-      <c r="AB78" s="1" t="str">
-        <f t="shared" ref="AB78" si="36">"SearchParameter-us-core-"&amp;LOWER((B78)&amp;"-"&amp;C78&amp;".html")</f>
+      <c r="AA78" s="5"/>
+      <c r="AB78" s="12"/>
+      <c r="AC78" s="1" t="str">
+        <f t="shared" ref="AC78" si="36">"SearchParameter-us-core-"&amp;LOWER((B78)&amp;"-"&amp;C78&amp;".html")</f>
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="79" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>75</v>
       </c>
@@ -11032,33 +11051,33 @@
         <f t="shared" ref="J79:J94" si="37">B79&amp;"."&amp;C79</f>
         <v>Device.patient</v>
       </c>
-      <c r="K79" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M79" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X79" s="1" t="s">
+      <c r="L79" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N79" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y79" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Y79" s="1" t="str">
+      <c r="Z79" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B79)&amp;"s for a patient, including implantable devices"</f>
         <v>support searching for all devices for a patient, including implantable devices</v>
       </c>
-      <c r="Z79" s="5" t="str">
+      <c r="AA79" s="5" t="str">
         <f>"GET [base]/"&amp;B79&amp;"?patient=1137192"</f>
         <v>GET [base]/Device?patient=1137192</v>
       </c>
-      <c r="AA79" s="12" t="str">
+      <c r="AB79" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B79&amp; " resources for the specified patient"</f>
         <v>Fetches a bundle of all Device resources for the specified patient</v>
       </c>
-      <c r="AB79" s="1" t="str">
-        <f t="shared" ref="AB79:AB90" si="38">"SearchParameter-us-core-"&amp;LOWER((B79)&amp;"-"&amp;C79&amp;".html")</f>
+      <c r="AC79" s="1" t="str">
+        <f t="shared" ref="AC79:AC90" si="38">"SearchParameter-us-core-"&amp;LOWER((B79)&amp;"-"&amp;C79&amp;".html")</f>
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>76</v>
       </c>
@@ -11091,20 +11110,20 @@
         <f t="shared" ref="J80" si="39">B80&amp;"."&amp;C80</f>
         <v>Device.type</v>
       </c>
-      <c r="K80" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M80" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z80" s="5"/>
-      <c r="AA80" s="12"/>
-      <c r="AB80" s="1" t="str">
+      <c r="L80" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA80" s="5"/>
+      <c r="AB80" s="12"/>
+      <c r="AC80" s="1" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-device-type.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>77</v>
       </c>
@@ -11137,28 +11156,28 @@
         <f t="shared" si="37"/>
         <v>Location.name</v>
       </c>
-      <c r="K81" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M81" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y81" s="1" t="s">
+      <c r="L81" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z81" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="Z81" s="7" t="s">
+      <c r="AA81" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="AA81" s="12" t="str">
+      <c r="AB81" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B81&amp; " resources that match the name"</f>
         <v>Fetches a bundle of all Location resources that match the name</v>
       </c>
-      <c r="AB81" t="str">
+      <c r="AC81" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>78</v>
       </c>
@@ -11191,28 +11210,28 @@
         <f t="shared" si="37"/>
         <v>Location.address</v>
       </c>
-      <c r="K82" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M82" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y82" s="1" t="s">
+      <c r="L82" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N82" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z82" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="Z82" s="7" t="s">
+      <c r="AA82" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="AA82" s="12" t="str">
+      <c r="AB82" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B82&amp; " resources that match the address string"</f>
         <v>Fetches a bundle of all Location resources that match the address string</v>
       </c>
-      <c r="AB82" t="str">
+      <c r="AC82" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>79</v>
       </c>
@@ -11245,28 +11264,28 @@
         <f t="shared" si="37"/>
         <v>Location.address-city</v>
       </c>
-      <c r="K83" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M83" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y83" s="1" t="s">
+      <c r="L83" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z83" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="Z83" s="7" t="s">
+      <c r="AA83" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="AA83" s="12" t="str">
+      <c r="AB83" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp; " resources for the city"</f>
         <v>Fetches a bundle of all Location resources for the city</v>
       </c>
-      <c r="AB83" t="str">
+      <c r="AC83" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>80</v>
       </c>
@@ -11299,28 +11318,28 @@
         <f t="shared" si="37"/>
         <v>Location.address-state</v>
       </c>
-      <c r="K84" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M84" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y84" s="1" t="s">
+      <c r="L84" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N84" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z84" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="Z84" s="7" t="s">
+      <c r="AA84" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="AA84" s="12" t="str">
+      <c r="AB84" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp; " resources for the state"</f>
         <v>Fetches a bundle of all Location resources for the state</v>
       </c>
-      <c r="AB84" t="str">
+      <c r="AC84" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>81</v>
       </c>
@@ -11353,28 +11372,28 @@
         <f t="shared" si="37"/>
         <v>Location.address-postalcode</v>
       </c>
-      <c r="K85" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M85" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y85" s="1" t="s">
+      <c r="L85" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N85" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z85" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="Z85" s="7" t="s">
+      <c r="AA85" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="AA85" s="12" t="str">
+      <c r="AB85" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B85&amp; " resources for the ZIP code"</f>
         <v>Fetches a bundle of all Location resources for the ZIP code</v>
       </c>
-      <c r="AB85" t="str">
+      <c r="AC85" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>82</v>
       </c>
@@ -11407,28 +11426,28 @@
         <f t="shared" si="37"/>
         <v>Organization.name</v>
       </c>
-      <c r="K86" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M86" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y86" s="1" t="s">
+      <c r="L86" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N86" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z86" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="Z86" s="7" t="s">
+      <c r="AA86" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="AA86" s="12" t="str">
+      <c r="AB86" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B86&amp; " resources that match the name"</f>
         <v>Fetches a bundle of all Organization resources that match the name</v>
       </c>
-      <c r="AB86" s="1" t="str">
+      <c r="AC86" s="1" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>83</v>
       </c>
@@ -11461,28 +11480,28 @@
         <f t="shared" si="37"/>
         <v>Organization.address</v>
       </c>
-      <c r="K87" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M87" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y87" s="1" t="s">
+      <c r="L87" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N87" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z87" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="Z87" s="7" t="s">
+      <c r="AA87" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="AA87" s="12" t="str">
+      <c r="AB87" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp; " resources that match the address string"</f>
         <v>Fetches a bundle of all Organization resources that match the address string</v>
       </c>
-      <c r="AB87" s="1" t="str">
+      <c r="AC87" s="1" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>84</v>
       </c>
@@ -11515,28 +11534,28 @@
         <f t="shared" si="37"/>
         <v>!Organization.address-city</v>
       </c>
-      <c r="K88" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M88" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y88" s="1" t="s">
+      <c r="L88" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N88" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z88" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="Z88" s="7" t="s">
+      <c r="AA88" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="AA88" s="12" t="str">
+      <c r="AB88" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp; " resources for the city"</f>
         <v>Fetches a bundle of all !Organization resources for the city</v>
       </c>
-      <c r="AB88" s="1" t="str">
+      <c r="AC88" s="1" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -11569,28 +11588,28 @@
         <f t="shared" si="37"/>
         <v>!Organization.adress-state</v>
       </c>
-      <c r="K89" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M89" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y89" s="1" t="s">
+      <c r="L89" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N89" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z89" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="Z89" s="7" t="s">
+      <c r="AA89" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="AA89" s="12" t="str">
+      <c r="AB89" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp; " resources for the state"</f>
         <v>Fetches a bundle of all !Organization resources for the state</v>
       </c>
-      <c r="AB89" s="1" t="str">
+      <c r="AC89" s="1" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>86</v>
       </c>
@@ -11623,28 +11642,28 @@
         <f t="shared" si="37"/>
         <v>!Organization.address-postalcode</v>
       </c>
-      <c r="K90" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M90" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y90" s="1" t="s">
+      <c r="L90" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N90" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z90" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="Z90" s="7" t="s">
+      <c r="AA90" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="AA90" s="12" t="str">
+      <c r="AB90" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp; " resources for the ZIP code"</f>
         <v>Fetches a bundle of all !Organization resources for the ZIP code</v>
       </c>
-      <c r="AB90" s="1" t="str">
+      <c r="AC90" s="1" t="str">
         <f t="shared" si="38"/>
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>87</v>
       </c>
@@ -11677,31 +11696,31 @@
         <f t="shared" si="37"/>
         <v>Practitioner.name</v>
       </c>
-      <c r="K91" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M91" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X91" s="1" t="s">
+      <c r="L91" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N91" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y91" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Y91" s="5" t="s">
+      <c r="Z91" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="Z91" s="7" t="s">
+      <c r="AA91" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="AA91" s="12" t="str">
+      <c r="AB91" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources matching the name"</f>
         <v>Fetches a bundle of all Practitioner resources matching the name</v>
       </c>
-      <c r="AB91" s="1" t="str">
-        <f t="shared" ref="AB91:AB92" si="40">"SearchParameter-us-core-"&amp;LOWER((B91)&amp;"-"&amp;SUBSTITUTE(C91,"_","")&amp;".html")</f>
+      <c r="AC91" s="1" t="str">
+        <f t="shared" ref="AC91:AC92" si="40">"SearchParameter-us-core-"&amp;LOWER((B91)&amp;"-"&amp;SUBSTITUTE(C91,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>88</v>
       </c>
@@ -11734,28 +11753,28 @@
         <f t="shared" si="37"/>
         <v>Practitioner.identifier</v>
       </c>
-      <c r="K92" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M92" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y92" s="5" t="s">
+      <c r="L92" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N92" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z92" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="Z92" s="7" t="s">
+      <c r="AA92" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="AA92" s="12" t="str">
+      <c r="AB92" s="12" t="str">
         <f>"Fetches a bundle containing any "&amp;B92&amp;" resources matching the identifier"</f>
         <v>Fetches a bundle containing any Practitioner resources matching the identifier</v>
       </c>
-      <c r="AB92" s="1" t="str">
+      <c r="AC92" s="1" t="str">
         <f t="shared" si="40"/>
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:29" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>89</v>
       </c>
@@ -11788,31 +11807,31 @@
         <f t="shared" si="37"/>
         <v>PractitionerRole.specialty</v>
       </c>
-      <c r="K93" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M93" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="V93" s="1" t="s">
+      <c r="L93" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N93" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W93" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="Y93" s="5" t="s">
+      <c r="Z93" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="Z93" s="7" t="s">
+      <c r="AA93" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="AA93" s="12" t="str">
+      <c r="AB93" s="12" t="str">
         <f>"Fetches a bundle containing  "&amp;B93&amp;" resources matching the specialty"</f>
         <v>Fetches a bundle containing  PractitionerRole resources matching the specialty</v>
       </c>
-      <c r="AB93" s="1" t="str">
-        <f t="shared" ref="AB93" si="41">"SearchParameter-us-core-"&amp;LOWER((B93)&amp;"-"&amp;SUBSTITUTE(C93,"_","")&amp;".html")</f>
+      <c r="AC93" s="1" t="str">
+        <f t="shared" ref="AC93" si="41">"SearchParameter-us-core-"&amp;LOWER((B93)&amp;"-"&amp;SUBSTITUTE(C93,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:29" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>90</v>
       </c>
@@ -11845,36 +11864,36 @@
         <f t="shared" si="37"/>
         <v>PractitionerRole.practitioner</v>
       </c>
-      <c r="K94" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M94" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="S94" s="1" t="s">
+      <c r="L94" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N94" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T94" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="V94" s="1" t="s">
+      <c r="W94" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="Y94" s="5" t="s">
+      <c r="Z94" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="Z94" s="7" t="s">
+      <c r="AA94" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="AA94" s="12" t="str">
+      <c r="AB94" s="12" t="str">
         <f>"Fetches a bundle containing  "&amp;B94&amp;" resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint."</f>
         <v>Fetches a bundle containing  PractitionerRole resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint.</v>
       </c>
-      <c r="AB94" t="str">
+      <c r="AC94" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B94)&amp;"-"&amp;SUBSTITUTE(C94,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB94" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA34">
+  <autoFilter ref="A1:AC94" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AB34">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>